<commit_message>
2022 Day 2 & 3
</commit_message>
<xml_diff>
--- a/2021/Day12 (INCOMPLETE).xlsx
+++ b/2021/Day12 (INCOMPLETE).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nfalero/Documents/Excel/Excel &amp; Financial Modelling/Advent-of-Code-Excel/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4578653-6743-B445-AB08-30E01FDD9079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7F2A23-5E1D-C240-9721-7212E3CA2A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17020" yWindow="760" windowWidth="16560" windowHeight="21580" activeTab="1" xr2:uid="{0286F73B-7DEB-7447-A9DB-423A598096A0}"/>
+    <workbookView xWindow="-25300" yWindow="600" windowWidth="25300" windowHeight="16360" activeTab="1" xr2:uid="{0286F73B-7DEB-7447-A9DB-423A598096A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Solutions" sheetId="2" r:id="rId1"/>
@@ -32,6 +32,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -577,7 +579,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>